<commit_message>
New version of links and structure excel
</commit_message>
<xml_diff>
--- a/thesis/SampleThesisStructure_ByJuhaniValimaki.xlsx
+++ b/thesis/SampleThesisStructure_ByJuhaniValimaki.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27218"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\public_html\thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\___GitRepos\share\thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_8FD2D9E85FBE1A37EB5C6A2A5F3B75619D5D9CF9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA848BDA-80F1-4B53-845E-DA9D0F590759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,16 +38,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
-    <t>by Juhani Välimäki</t>
-  </si>
-  <si>
-    <t>Version 11, 2019-04-10</t>
-  </si>
-  <si>
     <t>Cover page</t>
-  </si>
-  <si>
-    <t>(Tiivistelmä (Only in thesis written in Finnish))</t>
   </si>
   <si>
     <t>Abstract</t>
@@ -91,9 +93,6 @@
 =Thesis Reqs</t>
   </si>
   <si>
-    <t>Research problem / development goal, (research questions)</t>
-  </si>
-  <si>
     <t>(Research questions may go to Research plan in some academic type theses)</t>
   </si>
   <si>
@@ -157,9 +156,6 @@
     <t>Pre-existing</t>
   </si>
   <si>
-    <t>~ 9-15 pages</t>
-  </si>
-  <si>
     <t>Criticism with the sources</t>
   </si>
   <si>
@@ -220,9 +216,6 @@
       </rPr>
       <t>and the selection argumentation), normally 1-2 pages, only in rare cases more (e.g., if the research method theory presented here)</t>
     </r>
-  </si>
-  <si>
-    <t>=Research plan / Development plan. (Research questions)</t>
   </si>
   <si>
     <t>Understand the difference between Data gathering methods (e.g. questionnaires, semi-structured interviews) and data analysis methods.</t>
@@ -330,9 +323,6 @@
     <t>Validity of results</t>
   </si>
   <si>
-    <t>e.g. vs. time or scope of application</t>
-  </si>
-  <si>
     <t>Sources</t>
   </si>
   <si>
@@ -348,9 +338,6 @@
     <t>Learning</t>
   </si>
   <si>
-    <t>(0,5-1,5 pages)</t>
-  </si>
-  <si>
     <t>Further research/development</t>
   </si>
   <si>
@@ -363,21 +350,86 @@
     <t>Nothing new introduced, but the summary of the thesis PLUS possible findings. Not writing about the whole thesis</t>
   </si>
   <si>
-    <t>References (Let's not call it Bibliography! That's a bit like "Read more here")</t>
-  </si>
-  <si>
-    <t>In alphabetical order. Word (2007) 2010-&gt; has automatic reference management. (Or go pro and use RefWorks based on HH library instructions, or another similar professional service: Mendeley)</t>
-  </si>
-  <si>
-    <t>Appendices</t>
-  </si>
-  <si>
     <t>Appendix 1</t>
   </si>
   <si>
     <t>Appendix 2</t>
   </si>
   <si>
+    <t>Appendix 3</t>
+  </si>
+  <si>
+    <t>Appendix N</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note!!!</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Rememeber to look also at the secondary tab of the Thesis evaluation statement and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>criteria excel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sheet!!! Gives more ideas about what to write where.</t>
+    </r>
+  </si>
+  <si>
+    <t>Juhani Välimäki</t>
+  </si>
+  <si>
+    <t>(((Tiivistelmä. If thesis written in Finnish or author Finnish. In Swedish if Swedish-speaker. Similar to Abstract, just in another language. Maturity exam)))</t>
+  </si>
+  <si>
+    <t>Version 13, 2025-10-28</t>
+  </si>
+  <si>
+    <t>~ 10-20 pages</t>
+  </si>
+  <si>
+    <t>Sources "discussing": Brown, Smith, Brown, Jones, Jackson, Brown, …</t>
+  </si>
+  <si>
+    <t>=Research plan / Development plan. (((Research questions?))))</t>
+  </si>
+  <si>
+    <t>Research problem / development goal, research questions here?</t>
+  </si>
+  <si>
+    <t>Appendices / Liitteet</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Some of the appendices could be </t>
     </r>
@@ -390,32 +442,35 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>confidential.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Then the published thesis would only have one "abstract" page describing the nature and principles of the content, but not having the content.</t>
-    </r>
-  </si>
-  <si>
-    <t>Appendix 3</t>
-  </si>
-  <si>
-    <t>Appendix 4</t>
-  </si>
-  <si>
-    <t>Appendix 5</t>
-  </si>
-  <si>
-    <t>Appendix N</t>
-  </si>
-  <si>
+      <t>confidential</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Then the published thesis would only have one "abstract" page describing the nature and principles of the content, but not having the content.</t>
+    </r>
+  </si>
+  <si>
+    <t>References / Lähteet (Let's not call it Bibliography! That's a bit like "Read more here")</t>
+  </si>
+  <si>
+    <t>(1-1,5 pages)</t>
+  </si>
+  <si>
+    <t>e.g. vs. time or scope of application, utilizability of the results</t>
+  </si>
+  <si>
+    <t>RQuestions answered?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In alphabetical order. Recommendation: Use </t>
+    </r>
     <r>
       <rPr>
         <b/>
@@ -425,38 +480,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Note!!!</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Rememeber to look also at the secondary tab of the Thesis evaluation statement and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>criteria excel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sheet!!! Gives more ideas about what to write where.</t>
+      <t>Mendeley</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> based on HH library instructions. ((Word (2007) 2010-&gt; has also automatic reference management.))</t>
     </r>
   </si>
 </sst>
@@ -464,7 +498,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,7 +553,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -644,11 +678,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -704,6 +762,21 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -740,19 +813,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1062,386 +1129,384 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="68.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="73.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="70.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="75.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="B4" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" ht="30">
-      <c r="B5" s="1" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="38"/>
+      <c r="D4" s="37"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="31" t="s">
+      <c r="D7" s="11"/>
+      <c r="E7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="20" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="20"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="20"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="26" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="20"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="45">
-      <c r="A9" s="32"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="10" t="s">
+      <c r="D10" s="11"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="20"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D11" s="11"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="27"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="32"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="10" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="27"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="32"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="10" t="s">
+      <c r="E12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="27"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A12" s="32"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="10" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="20"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="20"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="28"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="13" t="s">
+      <c r="E14" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="20"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="32"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="13" t="s">
+      <c r="E15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="16" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="20"/>
+      <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="32"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="13" t="s">
+      <c r="C16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E16" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A16" s="32"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="3" t="s">
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A17" s="20"/>
+      <c r="B17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="13"/>
-      <c r="E16" s="17" t="s">
+      <c r="C17" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A17" s="32"/>
-      <c r="B17" s="1" t="s">
+      <c r="D17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="E17" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="6" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="34"/>
+    </row>
+    <row r="19" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="20"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="D19" s="5"/>
+      <c r="E19" s="35"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="20"/>
+      <c r="B20" s="24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="60">
-      <c r="A18" s="32"/>
-      <c r="B18" s="23" t="s">
+      <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="7" t="s">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="20"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="26" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="20"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="32"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="29"/>
-    </row>
-    <row r="20" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A20" s="32"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="5" t="s">
+      <c r="D22" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="20"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="20"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="30"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="32"/>
-      <c r="B21" s="19" t="s">
+      <c r="D24" s="6"/>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="20"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D25" s="6"/>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="26" t="s">
+      <c r="D26" s="6"/>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="20"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="32"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="1" t="s">
+      <c r="D27" s="6"/>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="20"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="27"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="32"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="1" t="s">
+      <c r="D28" s="6"/>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="20"/>
+      <c r="B29" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D29" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="27"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="32"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="2" t="s">
+    </row>
+    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="20"/>
+      <c r="B30" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="27"/>
-    </row>
-    <row r="25" spans="1:5" ht="30">
-      <c r="A25" s="32"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="32"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="27"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="32"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="27"/>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A28" s="32"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="28"/>
-    </row>
-    <row r="29" spans="1:5" ht="30">
-      <c r="A29" s="32"/>
-      <c r="B29" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
-      <c r="A30" s="32"/>
-      <c r="B30" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" s="19" t="s">
-        <v>55</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B32" s="24" t="s">
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" spans="2:4" ht="45">
-      <c r="B33" s="19"/>
+    <row r="33" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="24"/>
       <c r="C33" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="19"/>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B34" s="24"/>
       <c r="C34" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D34" s="1"/>
     </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="19"/>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B35" s="24"/>
       <c r="C35" s="1" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D35" s="1"/>
     </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="19"/>
-      <c r="C36" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="2:4">
-      <c r="B37" s="19"/>
-      <c r="C37" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="39" spans="2:4" ht="45.75" thickBot="1">
-      <c r="B39" s="9" t="s">
-        <v>63</v>
+    <row r="36" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="2:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B37" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A8:A30"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B21:B28"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="E21:E28"/>
+  <mergeCells count="10">
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="E20:E28"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="A7:A30"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B20:B28"/>
+    <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B17:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>